<commit_message>
IS ratio function changes
</commit_message>
<xml_diff>
--- a/ph_statistical_methods/tests/test_data/testdata_DSR_ISR.xlsx
+++ b/ph_statistical_methods/tests/test_data/testdata_DSR_ISR.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24326"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25601"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Annabel.Westermann\Documents\R\Projects\PHEindicatormethods\tests\testthat\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\karandeep.kaur\Desktop\ph\PH_statistical_methods\ph_statistical_methods\tests\test_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2350B830-A37B-42B4-BC7E-33646F468262}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7AE54A8A-CB63-44A5-8375-B03EA465788E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11620" tabRatio="719" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" tabRatio="719" firstSheet="1" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="testdata_multigroup" sheetId="16" r:id="rId1"/>
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="700" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="700" uniqueCount="65">
   <si>
     <t>0-4</t>
   </si>
@@ -219,6 +219,27 @@
   <si>
     <t>indirectly standardised ratio x 1</t>
   </si>
+  <si>
+    <t>Value</t>
+  </si>
+  <si>
+    <t>Statistic</t>
+  </si>
+  <si>
+    <t>Method</t>
+  </si>
+  <si>
+    <t>lower_95_ci</t>
+  </si>
+  <si>
+    <t>upper_95_ci</t>
+  </si>
+  <si>
+    <t>lower_99_8_ci</t>
+  </si>
+  <si>
+    <t>upper_99_8_ci</t>
+  </si>
 </sst>
 </file>
 
@@ -289,7 +310,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -299,6 +320,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.14999847407452621"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -316,7 +343,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="38">
+  <cellXfs count="39">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
@@ -423,6 +450,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -711,13 +739,13 @@
       <selection activeCell="G128" sqref="G128"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="14.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.140625" customWidth="1"/>
+    <col min="1" max="1" width="14.1796875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.1796875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1" s="16" t="s">
         <v>25</v>
       </c>
@@ -734,7 +762,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>23</v>
       </c>
@@ -751,7 +779,7 @@
         <v>636</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>23</v>
       </c>
@@ -768,7 +796,7 @@
         <v>558</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>23</v>
       </c>
@@ -785,7 +813,7 @@
         <v>609</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>23</v>
       </c>
@@ -802,7 +830,7 @@
         <v>543</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>23</v>
       </c>
@@ -819,7 +847,7 @@
         <v>384</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>23</v>
       </c>
@@ -836,7 +864,7 @@
         <v>594</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>23</v>
       </c>
@@ -853,7 +881,7 @@
         <v>669</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>23</v>
       </c>
@@ -870,7 +898,7 @@
         <v>843</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>23</v>
       </c>
@@ -887,7 +915,7 @@
         <v>660</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>23</v>
       </c>
@@ -904,7 +932,7 @@
         <v>576</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>23</v>
       </c>
@@ -921,7 +949,7 @@
         <v>606</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>23</v>
       </c>
@@ -938,7 +966,7 @@
         <v>522</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>23</v>
       </c>
@@ -955,7 +983,7 @@
         <v>426</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>23</v>
       </c>
@@ -972,7 +1000,7 @@
         <v>273</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>23</v>
       </c>
@@ -989,7 +1017,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>23</v>
       </c>
@@ -1006,7 +1034,7 @@
         <v>288</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>23</v>
       </c>
@@ -1023,7 +1051,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>23</v>
       </c>
@@ -1040,7 +1068,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
         <v>23</v>
       </c>
@@ -1057,7 +1085,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
         <v>24</v>
       </c>
@@ -1074,7 +1102,7 @@
         <v>636</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
         <v>24</v>
       </c>
@@ -1091,7 +1119,7 @@
         <v>558</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
         <v>24</v>
       </c>
@@ -1108,7 +1136,7 @@
         <v>609</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
         <v>24</v>
       </c>
@@ -1125,7 +1153,7 @@
         <v>543</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
         <v>24</v>
       </c>
@@ -1142,7 +1170,7 @@
         <v>384</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
         <v>24</v>
       </c>
@@ -1159,7 +1187,7 @@
         <v>594</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
         <v>24</v>
       </c>
@@ -1176,7 +1204,7 @@
         <v>669</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
         <v>24</v>
       </c>
@@ -1193,7 +1221,7 @@
         <v>843</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
         <v>24</v>
       </c>
@@ -1210,7 +1238,7 @@
         <v>660</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
         <v>24</v>
       </c>
@@ -1227,7 +1255,7 @@
         <v>576</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
         <v>24</v>
       </c>
@@ -1244,7 +1272,7 @@
         <v>606</v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
         <v>24</v>
       </c>
@@ -1261,7 +1289,7 @@
         <v>522</v>
       </c>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A33" t="s">
         <v>24</v>
       </c>
@@ -1278,7 +1306,7 @@
         <v>426</v>
       </c>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A34" t="s">
         <v>24</v>
       </c>
@@ -1295,7 +1323,7 @@
         <v>273</v>
       </c>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A35" t="s">
         <v>24</v>
       </c>
@@ -1312,7 +1340,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A36" t="s">
         <v>24</v>
       </c>
@@ -1329,7 +1357,7 @@
         <v>288</v>
       </c>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A37" t="s">
         <v>24</v>
       </c>
@@ -1346,7 +1374,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A38" t="s">
         <v>24</v>
       </c>
@@ -1363,7 +1391,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A39" t="s">
         <v>24</v>
       </c>
@@ -1380,7 +1408,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A40" t="s">
         <v>29</v>
       </c>
@@ -1397,7 +1425,7 @@
         <v>636</v>
       </c>
     </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A41" t="s">
         <v>29</v>
       </c>
@@ -1414,7 +1442,7 @@
         <v>558</v>
       </c>
     </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A42" t="s">
         <v>29</v>
       </c>
@@ -1431,7 +1459,7 @@
         <v>609</v>
       </c>
     </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A43" t="s">
         <v>29</v>
       </c>
@@ -1448,7 +1476,7 @@
         <v>543</v>
       </c>
     </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A44" t="s">
         <v>29</v>
       </c>
@@ -1465,7 +1493,7 @@
         <v>384</v>
       </c>
     </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A45" t="s">
         <v>29</v>
       </c>
@@ -1482,7 +1510,7 @@
         <v>594</v>
       </c>
     </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A46" t="s">
         <v>29</v>
       </c>
@@ -1499,7 +1527,7 @@
         <v>669</v>
       </c>
     </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A47" t="s">
         <v>29</v>
       </c>
@@ -1516,7 +1544,7 @@
         <v>843</v>
       </c>
     </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A48" t="s">
         <v>29</v>
       </c>
@@ -1533,7 +1561,7 @@
         <v>660</v>
       </c>
     </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A49" t="s">
         <v>29</v>
       </c>
@@ -1550,7 +1578,7 @@
         <v>576</v>
       </c>
     </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A50" t="s">
         <v>29</v>
       </c>
@@ -1567,7 +1595,7 @@
         <v>606</v>
       </c>
     </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A51" t="s">
         <v>29</v>
       </c>
@@ -1584,7 +1612,7 @@
         <v>522</v>
       </c>
     </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A52" t="s">
         <v>29</v>
       </c>
@@ -1601,7 +1629,7 @@
         <v>426</v>
       </c>
     </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A53" t="s">
         <v>29</v>
       </c>
@@ -1618,7 +1646,7 @@
         <v>273</v>
       </c>
     </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A54" t="s">
         <v>29</v>
       </c>
@@ -1635,7 +1663,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A55" t="s">
         <v>29</v>
       </c>
@@ -1652,7 +1680,7 @@
         <v>288</v>
       </c>
     </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A56" t="s">
         <v>29</v>
       </c>
@@ -1669,7 +1697,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A57" t="s">
         <v>29</v>
       </c>
@@ -1686,7 +1714,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A58" t="s">
         <v>29</v>
       </c>
@@ -1703,7 +1731,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A59" t="s">
         <v>23</v>
       </c>
@@ -1720,7 +1748,7 @@
         <v>668</v>
       </c>
     </row>
-    <row r="60" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A60" t="s">
         <v>23</v>
       </c>
@@ -1737,7 +1765,7 @@
         <v>586</v>
       </c>
     </row>
-    <row r="61" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A61" t="s">
         <v>23</v>
       </c>
@@ -1754,7 +1782,7 @@
         <v>639</v>
       </c>
     </row>
-    <row r="62" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A62" t="s">
         <v>23</v>
       </c>
@@ -1771,7 +1799,7 @@
         <v>570</v>
       </c>
     </row>
-    <row r="63" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A63" t="s">
         <v>23</v>
       </c>
@@ -1788,7 +1816,7 @@
         <v>403</v>
       </c>
     </row>
-    <row r="64" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A64" t="s">
         <v>23</v>
       </c>
@@ -1805,7 +1833,7 @@
         <v>624</v>
       </c>
     </row>
-    <row r="65" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A65" t="s">
         <v>23</v>
       </c>
@@ -1822,7 +1850,7 @@
         <v>702</v>
       </c>
     </row>
-    <row r="66" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A66" t="s">
         <v>23</v>
       </c>
@@ -1839,7 +1867,7 @@
         <v>885</v>
       </c>
     </row>
-    <row r="67" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A67" t="s">
         <v>23</v>
       </c>
@@ -1856,7 +1884,7 @@
         <v>693</v>
       </c>
     </row>
-    <row r="68" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A68" t="s">
         <v>23</v>
       </c>
@@ -1873,7 +1901,7 @@
         <v>605</v>
       </c>
     </row>
-    <row r="69" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A69" t="s">
         <v>23</v>
       </c>
@@ -1890,7 +1918,7 @@
         <v>636</v>
       </c>
     </row>
-    <row r="70" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A70" t="s">
         <v>23</v>
       </c>
@@ -1907,7 +1935,7 @@
         <v>548</v>
       </c>
     </row>
-    <row r="71" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A71" t="s">
         <v>23</v>
       </c>
@@ -1924,7 +1952,7 @@
         <v>447</v>
       </c>
     </row>
-    <row r="72" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A72" t="s">
         <v>23</v>
       </c>
@@ -1941,7 +1969,7 @@
         <v>287</v>
       </c>
     </row>
-    <row r="73" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A73" t="s">
         <v>23</v>
       </c>
@@ -1958,7 +1986,7 @@
         <v>315</v>
       </c>
     </row>
-    <row r="74" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A74" t="s">
         <v>23</v>
       </c>
@@ -1975,7 +2003,7 @@
         <v>302</v>
       </c>
     </row>
-    <row r="75" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A75" t="s">
         <v>23</v>
       </c>
@@ -1992,7 +2020,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="76" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A76" t="s">
         <v>23</v>
       </c>
@@ -2009,7 +2037,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="77" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A77" t="s">
         <v>23</v>
       </c>
@@ -2026,7 +2054,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="78" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A78" t="s">
         <v>24</v>
       </c>
@@ -2043,7 +2071,7 @@
         <v>668</v>
       </c>
     </row>
-    <row r="79" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A79" t="s">
         <v>24</v>
       </c>
@@ -2060,7 +2088,7 @@
         <v>586</v>
       </c>
     </row>
-    <row r="80" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A80" t="s">
         <v>24</v>
       </c>
@@ -2077,7 +2105,7 @@
         <v>639</v>
       </c>
     </row>
-    <row r="81" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A81" t="s">
         <v>24</v>
       </c>
@@ -2094,7 +2122,7 @@
         <v>570</v>
       </c>
     </row>
-    <row r="82" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A82" t="s">
         <v>24</v>
       </c>
@@ -2111,7 +2139,7 @@
         <v>403</v>
       </c>
     </row>
-    <row r="83" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A83" t="s">
         <v>24</v>
       </c>
@@ -2128,7 +2156,7 @@
         <v>624</v>
       </c>
     </row>
-    <row r="84" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A84" t="s">
         <v>24</v>
       </c>
@@ -2145,7 +2173,7 @@
         <v>702</v>
       </c>
     </row>
-    <row r="85" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A85" t="s">
         <v>24</v>
       </c>
@@ -2162,7 +2190,7 @@
         <v>885</v>
       </c>
     </row>
-    <row r="86" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A86" t="s">
         <v>24</v>
       </c>
@@ -2179,7 +2207,7 @@
         <v>693</v>
       </c>
     </row>
-    <row r="87" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A87" t="s">
         <v>24</v>
       </c>
@@ -2196,7 +2224,7 @@
         <v>605</v>
       </c>
     </row>
-    <row r="88" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A88" t="s">
         <v>24</v>
       </c>
@@ -2213,7 +2241,7 @@
         <v>636</v>
       </c>
     </row>
-    <row r="89" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A89" t="s">
         <v>24</v>
       </c>
@@ -2230,7 +2258,7 @@
         <v>548</v>
       </c>
     </row>
-    <row r="90" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A90" t="s">
         <v>24</v>
       </c>
@@ -2247,7 +2275,7 @@
         <v>447</v>
       </c>
     </row>
-    <row r="91" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A91" t="s">
         <v>24</v>
       </c>
@@ -2264,7 +2292,7 @@
         <v>287</v>
       </c>
     </row>
-    <row r="92" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A92" t="s">
         <v>24</v>
       </c>
@@ -2281,7 +2309,7 @@
         <v>315</v>
       </c>
     </row>
-    <row r="93" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A93" t="s">
         <v>24</v>
       </c>
@@ -2298,7 +2326,7 @@
         <v>302</v>
       </c>
     </row>
-    <row r="94" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A94" t="s">
         <v>24</v>
       </c>
@@ -2315,7 +2343,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="95" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A95" t="s">
         <v>24</v>
       </c>
@@ -2332,7 +2360,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="96" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A96" t="s">
         <v>24</v>
       </c>
@@ -2349,7 +2377,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="97" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A97" t="s">
         <v>29</v>
       </c>
@@ -2366,7 +2394,7 @@
         <v>668</v>
       </c>
     </row>
-    <row r="98" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A98" t="s">
         <v>29</v>
       </c>
@@ -2383,7 +2411,7 @@
         <v>586</v>
       </c>
     </row>
-    <row r="99" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A99" t="s">
         <v>29</v>
       </c>
@@ -2400,7 +2428,7 @@
         <v>639</v>
       </c>
     </row>
-    <row r="100" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A100" t="s">
         <v>29</v>
       </c>
@@ -2417,7 +2445,7 @@
         <v>570</v>
       </c>
     </row>
-    <row r="101" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A101" t="s">
         <v>29</v>
       </c>
@@ -2434,7 +2462,7 @@
         <v>403</v>
       </c>
     </row>
-    <row r="102" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A102" t="s">
         <v>29</v>
       </c>
@@ -2451,7 +2479,7 @@
         <v>624</v>
       </c>
     </row>
-    <row r="103" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A103" t="s">
         <v>29</v>
       </c>
@@ -2468,7 +2496,7 @@
         <v>702</v>
       </c>
     </row>
-    <row r="104" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A104" t="s">
         <v>29</v>
       </c>
@@ -2485,7 +2513,7 @@
         <v>885</v>
       </c>
     </row>
-    <row r="105" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A105" t="s">
         <v>29</v>
       </c>
@@ -2502,7 +2530,7 @@
         <v>693</v>
       </c>
     </row>
-    <row r="106" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A106" t="s">
         <v>29</v>
       </c>
@@ -2519,7 +2547,7 @@
         <v>605</v>
       </c>
     </row>
-    <row r="107" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A107" t="s">
         <v>29</v>
       </c>
@@ -2536,7 +2564,7 @@
         <v>636</v>
       </c>
     </row>
-    <row r="108" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A108" t="s">
         <v>29</v>
       </c>
@@ -2553,7 +2581,7 @@
         <v>548</v>
       </c>
     </row>
-    <row r="109" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A109" t="s">
         <v>29</v>
       </c>
@@ -2570,7 +2598,7 @@
         <v>447</v>
       </c>
     </row>
-    <row r="110" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A110" t="s">
         <v>29</v>
       </c>
@@ -2587,7 +2615,7 @@
         <v>287</v>
       </c>
     </row>
-    <row r="111" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A111" t="s">
         <v>29</v>
       </c>
@@ -2604,7 +2632,7 @@
         <v>315</v>
       </c>
     </row>
-    <row r="112" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A112" t="s">
         <v>29</v>
       </c>
@@ -2621,7 +2649,7 @@
         <v>302</v>
       </c>
     </row>
-    <row r="113" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A113" t="s">
         <v>29</v>
       </c>
@@ -2638,7 +2666,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="114" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A114" t="s">
         <v>29</v>
       </c>
@@ -2655,7 +2683,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="115" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A115" t="s">
         <v>29</v>
       </c>
@@ -2687,15 +2715,15 @@
       <selection activeCell="O17" sqref="O17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="10.85546875" style="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.28515625" style="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.85546875" style="2" bestFit="1" customWidth="1"/>
-    <col min="4" max="16384" width="9.140625" style="2"/>
+    <col min="1" max="1" width="10.81640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.26953125" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.81640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="16384" width="9.1796875" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>25</v>
       </c>
@@ -2706,7 +2734,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A2" s="3" t="s">
         <v>44</v>
       </c>
@@ -2719,7 +2747,7 @@
       <c r="E2" s="15"/>
       <c r="F2" s="15"/>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A3" s="3" t="s">
         <v>44</v>
       </c>
@@ -2730,7 +2758,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A4" s="3" t="s">
         <v>44</v>
       </c>
@@ -2741,7 +2769,7 @@
         <v>609</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A5" s="3" t="s">
         <v>44</v>
       </c>
@@ -2752,7 +2780,7 @@
         <v>543</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A6" s="3" t="s">
         <v>44</v>
       </c>
@@ -2763,7 +2791,7 @@
         <v>384</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A7" s="3" t="s">
         <v>44</v>
       </c>
@@ -2774,7 +2802,7 @@
         <v>594</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A8" s="3" t="s">
         <v>44</v>
       </c>
@@ -2785,7 +2813,7 @@
         <v>669</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A9" s="3" t="s">
         <v>44</v>
       </c>
@@ -2796,7 +2824,7 @@
         <v>843</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A10" s="3" t="s">
         <v>44</v>
       </c>
@@ -2807,7 +2835,7 @@
         <v>660</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A11" s="3" t="s">
         <v>44</v>
       </c>
@@ -2818,7 +2846,7 @@
         <v>576</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A12" s="3" t="s">
         <v>44</v>
       </c>
@@ -2829,7 +2857,7 @@
         <v>606</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A13" s="3" t="s">
         <v>44</v>
       </c>
@@ -2840,7 +2868,7 @@
         <v>522</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A14" s="3" t="s">
         <v>44</v>
       </c>
@@ -2851,7 +2879,7 @@
         <v>426</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A15" s="3" t="s">
         <v>44</v>
       </c>
@@ -2862,7 +2890,7 @@
         <v>273</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A16" s="3" t="s">
         <v>44</v>
       </c>
@@ -2873,7 +2901,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A17" s="3" t="s">
         <v>44</v>
       </c>
@@ -2884,7 +2912,7 @@
         <v>288</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A18" s="3" t="s">
         <v>44</v>
       </c>
@@ -2895,7 +2923,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A19" s="3" t="s">
         <v>44</v>
       </c>
@@ -2906,7 +2934,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A20" s="3" t="s">
         <v>44</v>
       </c>
@@ -2917,7 +2945,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A21" s="13" t="s">
         <v>45</v>
       </c>
@@ -2928,7 +2956,7 @@
         <v>636</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A22" s="13" t="s">
         <v>45</v>
       </c>
@@ -2939,7 +2967,7 @@
         <v>558</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A23" s="13" t="s">
         <v>45</v>
       </c>
@@ -2950,7 +2978,7 @@
         <v>609</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A24" s="13" t="s">
         <v>45</v>
       </c>
@@ -2961,7 +2989,7 @@
         <v>543</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A25" s="13" t="s">
         <v>45</v>
       </c>
@@ -2972,7 +3000,7 @@
         <v>384</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A26" s="13" t="s">
         <v>45</v>
       </c>
@@ -2983,7 +3011,7 @@
         <v>594</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A27" s="13" t="s">
         <v>45</v>
       </c>
@@ -2994,7 +3022,7 @@
         <v>669</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A28" s="13" t="s">
         <v>45</v>
       </c>
@@ -3005,7 +3033,7 @@
         <v>843</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A29" s="13" t="s">
         <v>45</v>
       </c>
@@ -3016,7 +3044,7 @@
         <v>660</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A30" s="13" t="s">
         <v>45</v>
       </c>
@@ -3027,7 +3055,7 @@
         <v>576</v>
       </c>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A31" s="13" t="s">
         <v>45</v>
       </c>
@@ -3038,7 +3066,7 @@
         <v>606</v>
       </c>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A32" s="13" t="s">
         <v>45</v>
       </c>
@@ -3049,7 +3077,7 @@
         <v>522</v>
       </c>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A33" s="13" t="s">
         <v>45</v>
       </c>
@@ -3060,7 +3088,7 @@
         <v>426</v>
       </c>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A34" s="13" t="s">
         <v>45</v>
       </c>
@@ -3071,7 +3099,7 @@
         <v>273</v>
       </c>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A35" s="13" t="s">
         <v>45</v>
       </c>
@@ -3082,7 +3110,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A36" s="13" t="s">
         <v>45</v>
       </c>
@@ -3093,7 +3121,7 @@
         <v>288</v>
       </c>
     </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A37" s="13" t="s">
         <v>45</v>
       </c>
@@ -3104,7 +3132,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A38" s="13" t="s">
         <v>45</v>
       </c>
@@ -3115,7 +3143,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A39" s="13" t="s">
         <v>45</v>
       </c>
@@ -3126,11 +3154,11 @@
         <v>207</v>
       </c>
     </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:3" x14ac:dyDescent="0.35">
       <c r="B40" s="4"/>
       <c r="C40" s="5"/>
     </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:3" x14ac:dyDescent="0.35">
       <c r="B41" s="4"/>
       <c r="C41" s="5"/>
     </row>
@@ -3148,15 +3176,15 @@
       <selection activeCell="K24" sqref="K24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="10.85546875" style="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.28515625" style="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="10.85546875" style="2" bestFit="1" customWidth="1"/>
-    <col min="5" max="16384" width="9.140625" style="2"/>
+    <col min="1" max="1" width="10.81640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.26953125" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="10.81640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="5" max="16384" width="9.1796875" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>22</v>
       </c>
@@ -3170,7 +3198,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A2" s="3" t="s">
         <v>0</v>
       </c>
@@ -3184,7 +3212,7 @@
         <v>5000</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A3" s="9" t="s">
         <v>1</v>
       </c>
@@ -3198,7 +3226,7 @@
         <v>5500</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A4" s="9" t="s">
         <v>2</v>
       </c>
@@ -3212,7 +3240,7 @@
         <v>5500</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A5" s="3" t="s">
         <v>3</v>
       </c>
@@ -3226,7 +3254,7 @@
         <v>5500</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A6" s="3" t="s">
         <v>4</v>
       </c>
@@ -3240,7 +3268,7 @@
         <v>6000</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A7" s="3" t="s">
         <v>5</v>
       </c>
@@ -3254,7 +3282,7 @@
         <v>6000</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A8" s="3" t="s">
         <v>6</v>
       </c>
@@ -3268,7 +3296,7 @@
         <v>6500</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A9" s="3" t="s">
         <v>7</v>
       </c>
@@ -3282,7 +3310,7 @@
         <v>7000</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A10" s="3" t="s">
         <v>8</v>
       </c>
@@ -3296,7 +3324,7 @@
         <v>7000</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A11" s="3" t="s">
         <v>9</v>
       </c>
@@ -3310,7 +3338,7 @@
         <v>7000</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A12" s="3" t="s">
         <v>10</v>
       </c>
@@ -3324,7 +3352,7 @@
         <v>7000</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A13" s="3" t="s">
         <v>11</v>
       </c>
@@ -3338,7 +3366,7 @@
         <v>6500</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A14" s="3" t="s">
         <v>12</v>
       </c>
@@ -3352,7 +3380,7 @@
         <v>6000</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A15" s="3" t="s">
         <v>13</v>
       </c>
@@ -3366,7 +3394,7 @@
         <v>5500</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A16" s="3" t="s">
         <v>14</v>
       </c>
@@ -3380,7 +3408,7 @@
         <v>5000</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A17" s="3" t="s">
         <v>15</v>
       </c>
@@ -3394,7 +3422,7 @@
         <v>4000</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A18" s="3" t="s">
         <v>16</v>
       </c>
@@ -3408,7 +3436,7 @@
         <v>2500</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A19" s="3" t="s">
         <v>17</v>
       </c>
@@ -3422,7 +3450,7 @@
         <v>1500</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A20" s="3" t="s">
         <v>18</v>
       </c>
@@ -3436,13 +3464,13 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A21" s="13"/>
       <c r="B21" s="7"/>
       <c r="C21" s="8"/>
       <c r="D21" s="14"/>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.35">
       <c r="B22" s="15"/>
     </row>
   </sheetData>
@@ -3455,16 +3483,16 @@
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:F58"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="I7" sqref="I7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.1796875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A1" s="16" t="s">
         <v>25</v>
       </c>
@@ -3484,7 +3512,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>23</v>
       </c>
@@ -3504,7 +3532,7 @@
         <v>50520</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>23</v>
       </c>
@@ -3524,7 +3552,7 @@
         <v>57173</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>23</v>
       </c>
@@ -3544,7 +3572,7 @@
         <v>60213</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>23</v>
       </c>
@@ -3564,7 +3592,7 @@
         <v>54659</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>23</v>
       </c>
@@ -3584,7 +3612,7 @@
         <v>44345</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>23</v>
       </c>
@@ -3604,7 +3632,7 @@
         <v>50128</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>23</v>
       </c>
@@ -3624,7 +3652,7 @@
         <v>62163</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>23</v>
       </c>
@@ -3644,7 +3672,7 @@
         <v>67423</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>23</v>
       </c>
@@ -3664,7 +3692,7 @@
         <v>62899</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>23</v>
       </c>
@@ -3684,7 +3712,7 @@
         <v>55463</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>23</v>
       </c>
@@ -3704,7 +3732,7 @@
         <v>60479</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>23</v>
       </c>
@@ -3724,7 +3752,7 @@
         <v>49974</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>23</v>
       </c>
@@ -3744,7 +3772,7 @@
         <v>44140</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>23</v>
       </c>
@@ -3764,7 +3792,7 @@
         <v>40888</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>23</v>
       </c>
@@ -3784,7 +3812,7 @@
         <v>37239</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>23</v>
       </c>
@@ -3804,7 +3832,7 @@
         <v>30819</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>23</v>
       </c>
@@ -3824,7 +3852,7 @@
         <v>18136</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>23</v>
       </c>
@@ -3844,7 +3872,7 @@
         <v>15325</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
         <v>23</v>
       </c>
@@ -3864,7 +3892,7 @@
         <v>13918</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
         <v>24</v>
       </c>
@@ -3884,7 +3912,7 @@
         <v>50520</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
         <v>24</v>
       </c>
@@ -3904,7 +3932,7 @@
         <v>57173</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
         <v>24</v>
       </c>
@@ -3924,7 +3952,7 @@
         <v>60213</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
         <v>24</v>
       </c>
@@ -3944,7 +3972,7 @@
         <v>54659</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
         <v>24</v>
       </c>
@@ -3964,7 +3992,7 @@
         <v>44345</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
         <v>24</v>
       </c>
@@ -3984,7 +4012,7 @@
         <v>50128</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
         <v>24</v>
       </c>
@@ -4004,7 +4032,7 @@
         <v>62163</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
         <v>24</v>
       </c>
@@ -4024,7 +4052,7 @@
         <v>67423</v>
       </c>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
         <v>24</v>
       </c>
@@ -4044,7 +4072,7 @@
         <v>62899</v>
       </c>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
         <v>24</v>
       </c>
@@ -4064,7 +4092,7 @@
         <v>55463</v>
       </c>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
         <v>24</v>
       </c>
@@ -4084,7 +4112,7 @@
         <v>60479</v>
       </c>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
         <v>24</v>
       </c>
@@ -4104,7 +4132,7 @@
         <v>49974</v>
       </c>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A33" t="s">
         <v>24</v>
       </c>
@@ -4124,7 +4152,7 @@
         <v>44140</v>
       </c>
     </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A34" t="s">
         <v>24</v>
       </c>
@@ -4144,7 +4172,7 @@
         <v>40888</v>
       </c>
     </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A35" t="s">
         <v>24</v>
       </c>
@@ -4164,7 +4192,7 @@
         <v>37239</v>
       </c>
     </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A36" t="s">
         <v>24</v>
       </c>
@@ -4184,7 +4212,7 @@
         <v>30819</v>
       </c>
     </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A37" t="s">
         <v>24</v>
       </c>
@@ -4204,7 +4232,7 @@
         <v>18136</v>
       </c>
     </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A38" t="s">
         <v>24</v>
       </c>
@@ -4224,7 +4252,7 @@
         <v>15325</v>
       </c>
     </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A39" t="s">
         <v>24</v>
       </c>
@@ -4244,7 +4272,7 @@
         <v>13918</v>
       </c>
     </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A40" t="s">
         <v>29</v>
       </c>
@@ -4264,7 +4292,7 @@
         <v>50520</v>
       </c>
     </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A41" t="s">
         <v>29</v>
       </c>
@@ -4284,7 +4312,7 @@
         <v>57173</v>
       </c>
     </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A42" t="s">
         <v>29</v>
       </c>
@@ -4295,7 +4323,7 @@
         <v>60213</v>
       </c>
     </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A43" t="s">
         <v>29</v>
       </c>
@@ -4315,7 +4343,7 @@
         <v>54659</v>
       </c>
     </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A44" t="s">
         <v>29</v>
       </c>
@@ -4335,7 +4363,7 @@
         <v>44345</v>
       </c>
     </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A45" t="s">
         <v>29</v>
       </c>
@@ -4355,7 +4383,7 @@
         <v>50128</v>
       </c>
     </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A46" t="s">
         <v>29</v>
       </c>
@@ -4375,7 +4403,7 @@
         <v>62163</v>
       </c>
     </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A47" t="s">
         <v>29</v>
       </c>
@@ -4395,7 +4423,7 @@
         <v>67423</v>
       </c>
     </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A48" t="s">
         <v>29</v>
       </c>
@@ -4415,7 +4443,7 @@
         <v>62899</v>
       </c>
     </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A49" t="s">
         <v>29</v>
       </c>
@@ -4435,7 +4463,7 @@
         <v>55463</v>
       </c>
     </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A50" t="s">
         <v>29</v>
       </c>
@@ -4455,7 +4483,7 @@
         <v>60479</v>
       </c>
     </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A51" t="s">
         <v>29</v>
       </c>
@@ -4475,7 +4503,7 @@
         <v>49974</v>
       </c>
     </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A52" t="s">
         <v>29</v>
       </c>
@@ -4495,7 +4523,7 @@
         <v>44140</v>
       </c>
     </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A53" t="s">
         <v>29</v>
       </c>
@@ -4515,7 +4543,7 @@
         <v>40888</v>
       </c>
     </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A54" t="s">
         <v>29</v>
       </c>
@@ -4535,7 +4563,7 @@
         <v>37239</v>
       </c>
     </row>
-    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A55" t="s">
         <v>29</v>
       </c>
@@ -4555,7 +4583,7 @@
         <v>30819</v>
       </c>
     </row>
-    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A56" t="s">
         <v>29</v>
       </c>
@@ -4575,7 +4603,7 @@
         <v>18136</v>
       </c>
     </row>
-    <row r="57" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A57" t="s">
         <v>29</v>
       </c>
@@ -4595,7 +4623,7 @@
         <v>15325</v>
       </c>
     </row>
-    <row r="58" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A58" t="s">
         <v>29</v>
       </c>
@@ -4629,13 +4657,13 @@
       <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="18" customWidth="1"/>
-    <col min="2" max="2" width="10.7109375" customWidth="1"/>
+    <col min="2" max="2" width="10.7265625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A1" s="16" t="s">
         <v>25</v>
       </c>
@@ -4643,7 +4671,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>23</v>
       </c>
@@ -4651,7 +4679,7 @@
         <v>895</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>24</v>
       </c>
@@ -4665,7 +4693,7 @@
       <c r="J3" s="16"/>
       <c r="K3" s="16"/>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>29</v>
       </c>
@@ -4688,12 +4716,12 @@
       <selection activeCell="I56" sqref="I56"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.1796875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A1" s="16" t="s">
         <v>25</v>
       </c>
@@ -4707,7 +4735,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>23</v>
       </c>
@@ -4721,7 +4749,7 @@
         <v>636</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>23</v>
       </c>
@@ -4735,7 +4763,7 @@
         <v>558</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>23</v>
       </c>
@@ -4749,7 +4777,7 @@
         <v>609</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>23</v>
       </c>
@@ -4763,7 +4791,7 @@
         <v>543</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>23</v>
       </c>
@@ -4777,7 +4805,7 @@
         <v>384</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>23</v>
       </c>
@@ -4791,7 +4819,7 @@
         <v>594</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>23</v>
       </c>
@@ -4805,7 +4833,7 @@
         <v>669</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>23</v>
       </c>
@@ -4819,7 +4847,7 @@
         <v>843</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>23</v>
       </c>
@@ -4833,7 +4861,7 @@
         <v>660</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>23</v>
       </c>
@@ -4847,7 +4875,7 @@
         <v>576</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>23</v>
       </c>
@@ -4861,7 +4889,7 @@
         <v>606</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>23</v>
       </c>
@@ -4875,7 +4903,7 @@
         <v>522</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>23</v>
       </c>
@@ -4889,7 +4917,7 @@
         <v>426</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>23</v>
       </c>
@@ -4903,7 +4931,7 @@
         <v>273</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>23</v>
       </c>
@@ -4917,7 +4945,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>23</v>
       </c>
@@ -4931,7 +4959,7 @@
         <v>288</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>23</v>
       </c>
@@ -4945,7 +4973,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>23</v>
       </c>
@@ -4959,7 +4987,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
         <v>23</v>
       </c>
@@ -4973,7 +5001,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
         <v>24</v>
       </c>
@@ -4987,7 +5015,7 @@
         <v>636</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
         <v>24</v>
       </c>
@@ -5001,7 +5029,7 @@
         <v>558</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
         <v>24</v>
       </c>
@@ -5015,7 +5043,7 @@
         <v>609</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
         <v>24</v>
       </c>
@@ -5029,7 +5057,7 @@
         <v>543</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
         <v>24</v>
       </c>
@@ -5043,7 +5071,7 @@
         <v>384</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
         <v>24</v>
       </c>
@@ -5057,7 +5085,7 @@
         <v>594</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
         <v>24</v>
       </c>
@@ -5071,7 +5099,7 @@
         <v>669</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
         <v>24</v>
       </c>
@@ -5085,7 +5113,7 @@
         <v>843</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
         <v>24</v>
       </c>
@@ -5099,7 +5127,7 @@
         <v>660</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
         <v>24</v>
       </c>
@@ -5113,7 +5141,7 @@
         <v>576</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
         <v>24</v>
       </c>
@@ -5127,7 +5155,7 @@
         <v>606</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
         <v>24</v>
       </c>
@@ -5141,7 +5169,7 @@
         <v>522</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A33" t="s">
         <v>24</v>
       </c>
@@ -5155,7 +5183,7 @@
         <v>426</v>
       </c>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A34" t="s">
         <v>24</v>
       </c>
@@ -5169,7 +5197,7 @@
         <v>273</v>
       </c>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A35" t="s">
         <v>24</v>
       </c>
@@ -5183,7 +5211,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A36" t="s">
         <v>24</v>
       </c>
@@ -5197,7 +5225,7 @@
         <v>288</v>
       </c>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A37" t="s">
         <v>24</v>
       </c>
@@ -5211,7 +5239,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A38" t="s">
         <v>24</v>
       </c>
@@ -5225,7 +5253,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A39" t="s">
         <v>24</v>
       </c>
@@ -5239,7 +5267,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A40" t="s">
         <v>29</v>
       </c>
@@ -5253,7 +5281,7 @@
         <v>636</v>
       </c>
     </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A41" t="s">
         <v>29</v>
       </c>
@@ -5267,7 +5295,7 @@
         <v>558</v>
       </c>
     </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A42" t="s">
         <v>29</v>
       </c>
@@ -5278,7 +5306,7 @@
         <v>609</v>
       </c>
     </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A43" t="s">
         <v>29</v>
       </c>
@@ -5292,7 +5320,7 @@
         <v>543</v>
       </c>
     </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A44" t="s">
         <v>29</v>
       </c>
@@ -5306,7 +5334,7 @@
         <v>384</v>
       </c>
     </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A45" t="s">
         <v>29</v>
       </c>
@@ -5320,7 +5348,7 @@
         <v>594</v>
       </c>
     </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A46" t="s">
         <v>29</v>
       </c>
@@ -5334,7 +5362,7 @@
         <v>669</v>
       </c>
     </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A47" t="s">
         <v>29</v>
       </c>
@@ -5348,7 +5376,7 @@
         <v>843</v>
       </c>
     </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A48" t="s">
         <v>29</v>
       </c>
@@ -5362,7 +5390,7 @@
         <v>660</v>
       </c>
     </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A49" t="s">
         <v>29</v>
       </c>
@@ -5376,7 +5404,7 @@
         <v>576</v>
       </c>
     </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A50" t="s">
         <v>29</v>
       </c>
@@ -5390,7 +5418,7 @@
         <v>606</v>
       </c>
     </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A51" t="s">
         <v>29</v>
       </c>
@@ -5404,7 +5432,7 @@
         <v>522</v>
       </c>
     </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A52" t="s">
         <v>29</v>
       </c>
@@ -5418,7 +5446,7 @@
         <v>426</v>
       </c>
     </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A53" t="s">
         <v>29</v>
       </c>
@@ -5432,7 +5460,7 @@
         <v>273</v>
       </c>
     </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A54" t="s">
         <v>29</v>
       </c>
@@ -5446,7 +5474,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A55" t="s">
         <v>29</v>
       </c>
@@ -5460,7 +5488,7 @@
         <v>288</v>
       </c>
     </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A56" t="s">
         <v>29</v>
       </c>
@@ -5474,7 +5502,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A57" t="s">
         <v>29</v>
       </c>
@@ -5488,7 +5516,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A58" t="s">
         <v>29</v>
       </c>
@@ -5517,15 +5545,15 @@
       <selection activeCell="I26" sqref="I26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="10.85546875" style="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.28515625" style="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="10.85546875" style="2" bestFit="1" customWidth="1"/>
-    <col min="5" max="16384" width="9.140625" style="2"/>
+    <col min="1" max="1" width="10.81640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.26953125" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="10.81640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="5" max="16384" width="9.1796875" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>22</v>
       </c>
@@ -5539,7 +5567,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A2" s="3" t="s">
         <v>0</v>
       </c>
@@ -5553,7 +5581,7 @@
         <v>8000</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A3" s="9" t="s">
         <v>1</v>
       </c>
@@ -5567,7 +5595,7 @@
         <v>7000</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A4" s="9" t="s">
         <v>2</v>
       </c>
@@ -5581,7 +5609,7 @@
         <v>7000</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A5" s="3" t="s">
         <v>3</v>
       </c>
@@ -5595,7 +5623,7 @@
         <v>7000</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A6" s="3" t="s">
         <v>4</v>
       </c>
@@ -5609,7 +5637,7 @@
         <v>7000</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A7" s="3" t="s">
         <v>5</v>
       </c>
@@ -5623,7 +5651,7 @@
         <v>7000</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A8" s="3" t="s">
         <v>6</v>
       </c>
@@ -5637,7 +5665,7 @@
         <v>7000</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A9" s="3" t="s">
         <v>7</v>
       </c>
@@ -5651,7 +5679,7 @@
         <v>7000</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A10" s="3" t="s">
         <v>8</v>
       </c>
@@ -5665,7 +5693,7 @@
         <v>7000</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A11" s="3" t="s">
         <v>9</v>
       </c>
@@ -5679,7 +5707,7 @@
         <v>7000</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A12" s="3" t="s">
         <v>10</v>
       </c>
@@ -5693,7 +5721,7 @@
         <v>7000</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A13" s="3" t="s">
         <v>11</v>
       </c>
@@ -5707,7 +5735,7 @@
         <v>6000</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A14" s="3" t="s">
         <v>12</v>
       </c>
@@ -5721,7 +5749,7 @@
         <v>5000</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A15" s="3" t="s">
         <v>13</v>
       </c>
@@ -5735,7 +5763,7 @@
         <v>4000</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A16" s="3" t="s">
         <v>14</v>
       </c>
@@ -5749,7 +5777,7 @@
         <v>3000</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A17" s="3" t="s">
         <v>15</v>
       </c>
@@ -5763,7 +5791,7 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A18" s="3" t="s">
         <v>16</v>
       </c>
@@ -5777,7 +5805,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A19" s="3" t="s">
         <v>30</v>
       </c>
@@ -5791,19 +5819,19 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A20" s="3"/>
       <c r="B20" s="4"/>
       <c r="C20" s="5"/>
       <c r="D20" s="6"/>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A21" s="13"/>
       <c r="B21" s="7"/>
       <c r="C21" s="8"/>
       <c r="D21" s="14"/>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.35">
       <c r="B22" s="15"/>
     </row>
   </sheetData>
@@ -5821,9 +5849,9 @@
       <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A1" s="16" t="s">
         <v>22</v>
       </c>
@@ -5835,7 +5863,7 @@
       </c>
       <c r="D1" s="16"/>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -5846,7 +5874,7 @@
         <v>50520</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -5857,7 +5885,7 @@
         <v>57173</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -5868,7 +5896,7 @@
         <v>60213</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>3</v>
       </c>
@@ -5879,7 +5907,7 @@
         <v>54659</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>4</v>
       </c>
@@ -5890,7 +5918,7 @@
         <v>44345</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>5</v>
       </c>
@@ -5901,7 +5929,7 @@
         <v>50128</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>6</v>
       </c>
@@ -5912,7 +5940,7 @@
         <v>62163</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>7</v>
       </c>
@@ -5923,7 +5951,7 @@
         <v>67423</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>8</v>
       </c>
@@ -5934,7 +5962,7 @@
         <v>62899</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>9</v>
       </c>
@@ -5945,7 +5973,7 @@
         <v>55463</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>10</v>
       </c>
@@ -5956,7 +5984,7 @@
         <v>60479</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>11</v>
       </c>
@@ -5967,7 +5995,7 @@
         <v>49974</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>12</v>
       </c>
@@ -5978,7 +6006,7 @@
         <v>44140</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>13</v>
       </c>
@@ -5989,7 +6017,7 @@
         <v>40888</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>14</v>
       </c>
@@ -6000,7 +6028,7 @@
         <v>37239</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>15</v>
       </c>
@@ -6011,7 +6039,7 @@
         <v>30819</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>16</v>
       </c>
@@ -6022,7 +6050,7 @@
         <v>18136</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>17</v>
       </c>
@@ -6033,7 +6061,7 @@
         <v>15325</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
         <v>18</v>
       </c>
@@ -6054,22 +6082,22 @@
   <sheetPr codeName="Sheet6"/>
   <dimension ref="A1:K17"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="J20" sqref="J20"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H15" sqref="H15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="2" width="14.140625" customWidth="1"/>
-    <col min="3" max="4" width="9.140625" style="18"/>
+    <col min="1" max="2" width="14.1796875" customWidth="1"/>
+    <col min="3" max="4" width="9.1796875" style="18"/>
     <col min="5" max="6" width="12" style="18" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="12" style="22" bestFit="1" customWidth="1"/>
     <col min="8" max="9" width="12" style="22" customWidth="1"/>
-    <col min="10" max="10" width="38.5703125" style="33" customWidth="1"/>
-    <col min="11" max="11" width="9.140625" style="34"/>
+    <col min="10" max="10" width="38.54296875" style="33" customWidth="1"/>
+    <col min="11" max="11" width="9.1796875" style="34"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A1" s="16" t="s">
         <v>25</v>
       </c>
@@ -6083,28 +6111,28 @@
         <v>41</v>
       </c>
       <c r="E1" s="17" t="s">
-        <v>42</v>
-      </c>
-      <c r="F1" s="17" t="s">
-        <v>50</v>
-      </c>
-      <c r="G1" s="17" t="s">
-        <v>51</v>
-      </c>
-      <c r="H1" s="17" t="s">
-        <v>52</v>
-      </c>
-      <c r="I1" s="17" t="s">
-        <v>53</v>
+        <v>58</v>
+      </c>
+      <c r="F1" s="38" t="s">
+        <v>61</v>
+      </c>
+      <c r="G1" s="38" t="s">
+        <v>62</v>
+      </c>
+      <c r="H1" s="38" t="s">
+        <v>63</v>
+      </c>
+      <c r="I1" s="38" t="s">
+        <v>64</v>
       </c>
       <c r="J1" s="27" t="s">
-        <v>34</v>
+        <v>59</v>
       </c>
       <c r="K1" s="28" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="2" spans="1:11" s="31" customFormat="1" x14ac:dyDescent="0.25">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" s="31" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A2" s="31" t="s">
         <v>23</v>
       </c>
@@ -6139,7 +6167,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="3" spans="1:11" s="31" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" s="31" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A3" s="31" t="s">
         <v>24</v>
       </c>
@@ -6174,7 +6202,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="4" spans="1:11" s="31" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" s="31" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A4" s="31" t="s">
         <v>29</v>
       </c>
@@ -6209,7 +6237,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="5" spans="1:11" s="31" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11" s="31" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A5" s="31" t="s">
         <v>23</v>
       </c>
@@ -6244,7 +6272,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="6" spans="1:11" s="31" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11" s="31" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A6" s="31" t="s">
         <v>24</v>
       </c>
@@ -6279,7 +6307,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="7" spans="1:11" s="25" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:11" s="25" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A7" s="31" t="s">
         <v>29</v>
       </c>
@@ -6314,7 +6342,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="8" spans="1:11" s="31" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:11" s="31" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A8" s="31" t="s">
         <v>23</v>
       </c>
@@ -6346,7 +6374,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="9" spans="1:11" s="31" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:11" s="31" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A9" s="31" t="s">
         <v>24</v>
       </c>
@@ -6378,7 +6406,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="10" spans="1:11" s="26" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:11" s="26" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A10" s="34" t="s">
         <v>29</v>
       </c>
@@ -6411,7 +6439,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="11" spans="1:11" s="34" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:11" s="34" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A11" s="34" t="s">
         <v>23</v>
       </c>
@@ -6443,7 +6471,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="12" spans="1:11" s="34" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:11" s="34" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A12" s="34" t="s">
         <v>24</v>
       </c>
@@ -6475,7 +6503,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="13" spans="1:11" s="26" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:11" s="26" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A13" s="34" t="s">
         <v>29</v>
       </c>
@@ -6508,7 +6536,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="14" spans="1:11" s="34" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:11" s="34" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A14" s="34" t="s">
         <v>44</v>
       </c>
@@ -6539,7 +6567,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="15" spans="1:11" s="34" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:11" s="34" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A15" s="34" t="s">
         <v>45</v>
       </c>
@@ -6570,7 +6598,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="16" spans="1:11" s="34" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:11" s="34" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A16" s="34" t="s">
         <v>44</v>
       </c>
@@ -6599,7 +6627,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="17" spans="1:11" s="34" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:11" s="34" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A17" s="34" t="s">
         <v>45</v>
       </c>
@@ -6643,18 +6671,18 @@
       <selection activeCell="G18" sqref="G18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="14.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="14.140625" customWidth="1"/>
-    <col min="4" max="4" width="9.140625" style="18"/>
+    <col min="1" max="1" width="14.1796875" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="14.1796875" customWidth="1"/>
+    <col min="4" max="4" width="9.1796875" style="18"/>
     <col min="5" max="6" width="12" style="18" bestFit="1" customWidth="1"/>
     <col min="7" max="8" width="12" style="18" customWidth="1"/>
     <col min="9" max="9" width="12" style="24" customWidth="1"/>
     <col min="10" max="10" width="11" style="18" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A1" s="16" t="s">
         <v>25</v>
       </c>
@@ -6686,7 +6714,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>23</v>
       </c>
@@ -6718,7 +6746,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>24</v>
       </c>
@@ -6750,7 +6778,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>29</v>
       </c>
@@ -6767,7 +6795,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>31</v>
       </c>
@@ -6799,7 +6827,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>23</v>
       </c>
@@ -6831,7 +6859,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>24</v>
       </c>
@@ -6863,7 +6891,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>29</v>
       </c>
@@ -6880,7 +6908,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>31</v>
       </c>
@@ -6927,15 +6955,15 @@
       <selection activeCell="F25" sqref="F25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="10.85546875" style="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.28515625" style="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="10.85546875" style="2" bestFit="1" customWidth="1"/>
-    <col min="5" max="16384" width="9.140625" style="2"/>
+    <col min="1" max="1" width="10.81640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.26953125" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="10.81640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="5" max="16384" width="9.1796875" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>22</v>
       </c>
@@ -6949,7 +6977,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A2" s="3" t="s">
         <v>0</v>
       </c>
@@ -6963,7 +6991,7 @@
         <v>5000</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A3" s="9" t="s">
         <v>1</v>
       </c>
@@ -6977,7 +7005,7 @@
         <v>5500</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A4" s="9" t="s">
         <v>2</v>
       </c>
@@ -6991,7 +7019,7 @@
         <v>5500</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A5" s="3" t="s">
         <v>3</v>
       </c>
@@ -7005,7 +7033,7 @@
         <v>5500</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A6" s="3" t="s">
         <v>4</v>
       </c>
@@ -7019,7 +7047,7 @@
         <v>6000</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A7" s="3" t="s">
         <v>5</v>
       </c>
@@ -7033,7 +7061,7 @@
         <v>6000</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A8" s="3" t="s">
         <v>6</v>
       </c>
@@ -7047,7 +7075,7 @@
         <v>6500</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A9" s="3" t="s">
         <v>7</v>
       </c>
@@ -7061,7 +7089,7 @@
         <v>7000</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A10" s="3" t="s">
         <v>8</v>
       </c>
@@ -7075,7 +7103,7 @@
         <v>7000</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A11" s="3" t="s">
         <v>9</v>
       </c>
@@ -7089,7 +7117,7 @@
         <v>7000</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A12" s="3" t="s">
         <v>10</v>
       </c>
@@ -7103,7 +7131,7 @@
         <v>7000</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A13" s="3" t="s">
         <v>11</v>
       </c>
@@ -7117,7 +7145,7 @@
         <v>6500</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A14" s="3" t="s">
         <v>12</v>
       </c>
@@ -7131,7 +7159,7 @@
         <v>6000</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A15" s="3" t="s">
         <v>13</v>
       </c>
@@ -7145,7 +7173,7 @@
         <v>5500</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A16" s="3" t="s">
         <v>14</v>
       </c>
@@ -7159,7 +7187,7 @@
         <v>5000</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A17" s="3" t="s">
         <v>15</v>
       </c>
@@ -7173,7 +7201,7 @@
         <v>4000</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A18" s="3" t="s">
         <v>16</v>
       </c>
@@ -7187,7 +7215,7 @@
         <v>2500</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A19" s="3" t="s">
         <v>17</v>
       </c>
@@ -7201,7 +7229,7 @@
         <v>1500</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A20" s="3" t="s">
         <v>18</v>
       </c>
@@ -7215,13 +7243,13 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A21" s="13"/>
       <c r="B21" s="7"/>
       <c r="C21" s="8"/>
       <c r="D21" s="14"/>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.35">
       <c r="B22" s="15"/>
     </row>
   </sheetData>

</xml_diff>